<commit_message>
feat: add mountains seed data file.
</commit_message>
<xml_diff>
--- a/prisma/seeds/mountains.xlsx
+++ b/prisma/seeds/mountains.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11460" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -2717,7 +2717,7 @@
   <dimension ref="A1:J89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6" defaultRowHeight="14.25" customHeight="1"/>
@@ -2730,7 +2730,7 @@
     <col min="6" max="6" width="26" customWidth="1"/>
     <col min="7" max="7" width="21.8571428571429" customWidth="1"/>
     <col min="8" max="8" width="18.5714285714286" customWidth="1"/>
-    <col min="9" max="9" width="15.8571428571429" customWidth="1"/>
+    <col min="9" max="9" width="41.8571428571429" customWidth="1"/>
     <col min="10" max="10" width="18.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>